<commit_message>
updated data layers for LSP
</commit_message>
<xml_diff>
--- a/prep_whi/TR/wh_mma.xlsx
+++ b/prep_whi/TR/wh_mma.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28615"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents and Settings\eschemmel\Documents\github\WH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eschemmel/Documents/github/WHI/prep_whi/TR/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25120" windowHeight="12220" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="North" sheetId="1" r:id="rId1"/>
     <sheet name="area_west_hawaii" sheetId="3" r:id="rId2"/>
     <sheet name="South" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -538,7 +544,7 @@
     <t>HAR 13-58</t>
   </si>
   <si>
-    <t>Kona Coast” refers to the following four Fisheries Management Area Zones on the southwestern portion of Hawai‘i, each bounded by two lines extending seaward at right angles from shore and marked by signs on shore: (a) the “Wawāloli Zone”, from	To catch fish in the Zones with legal fishing gear for personal consumption.	To collect any aquarium fish within the Zones. To engage in fish feeding within the Zones, except for ‘ōpelu fishing.	http://dlnr.hawaii.gov/dar/files/2014/05/ch58.pdf	N/A	FMA	Fisheries Management Area	{8a932d40-796b-4f50-a9b6-de6e3f661352}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	2351774.23805	0_x000D_
+    <t>Kona Coast” refers to the following four Fisheries Management Area Zones on the southwestern portion of Hawai‘i, each bounded by two lines extending seaward at right angles from shore and marked by signs on shore: (a) the “Wawāloli Zone”, from	To catch fish in the Zones with legal fishing gear for personal consumption.	To collect any aquarium fish within the Zones. To engage in fish feeding within the Zones, except for ‘ōpelu fishing.	http://dlnr.hawaii.gov/dar/files/2014/05/ch58.pdf	N/A	FMA	Fisheries Management Area	{8a932d40-796b-4f50-a9b6-de6e3f661352}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	2351774.23805	0
 12	Polygon	29	Kona Coast Fisheries Management Area: Wawāloli	Kona Coast FMA: Wawaloli	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#kona-coast	HAR 13-58	Kona Coast” refers to the following four Fisheries Management Area Zones on the southwestern portion of Hawai‘i, each bounded by two lines extending seaward at right angles from shore and marked by signs on shore: (a) the “Wawāloli Zone”, from</t>
   </si>
   <si>
@@ -560,16 +566,16 @@
     <t>Kona Coast FMA: Papawai Bay</t>
   </si>
   <si>
-    <t>Kona Coast” refers to the following four Fisheries Management Area Zones on the southwestern portion of Hawai‘i, each bounded by two lines extending seaward at right angles from shore and marked by signs on shore: (a) the “Wawāloli Zone”, from	To catch fish in the Zones with legal fishing gear for personal consumption.	To collect any aquarium fish within the Zones. To engage in fish feeding within the Zones, except for ‘ōpelu fishing.	http://dlnr.hawaii.gov/dar/files/2014/05/ch58.pdf	N/A	FMA	Fisheries Management Area	{89c305aa-b0ed-41f5-92b0-ab311c3d5581}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	875909.246146	0_x000D_
-14	Polygon	43	West Hawai‘i Regional Fisheries Management Area: Ho‘okena	West Hawaii Regional FMA: Hookena	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#west-hawaii-regional-fishery-management-area	HAR 13-60.4	The West Hawai‘i Regional Fishery Management Area (FRA) extends along the west coast of the Island of Hawaii from Ka Lae, Ka‘ū (South Point) to ‘Upolu Point, North Kohala, and from the highwater mark on shore seaward to the limit of the State’s	All types of fishing, except as indicated in prohibited activities below.	To take, kill, possess, sell, or offer for sale, any specimen of the following: Hawaiian stingray, broad stingray, pelagic stingray, spotted eagle ray, blacktip reef shark, gray reef shark, whitetip reef shark, tiger shark, whale shark, horned helmet, an	http://dlnr.hawaii.gov/dar/files/2014/05/ch60.4.pdf	N/A	FMA	Fish Replenishment Area	{001f30aa-dd58-4b6c-b2e7-1bc7cf404eb4}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	6274248.7927	0_x000D_
-15	Polygon	20	South Kona (Miloli‘i) ‘Opelu Management Area	South Kona Opelu Mgmt Area	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#south-kona-milolii	HAR 13-95-18, HRS 188-22.7	The waters off the coast of South Kona between the Ki‘ilae-Kēōkea boundary and the Kapua-Kaulanamauna boundary.	N/A	To fish for or take opelu with fish or animal bait, except with hook and line.	http://dlnr.hawaii.gov/dar/files/2016/03/ch95.pdf	http://www.capitol.hawaii.gov/hrscurrent/Vol03_Ch0121-0200D/HRS0188/HRS_0188-0022_0007.htm	FMA	Opelu Management Area	{add90ebb-5d87-4dad-9c54-c88ca170499c}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	24866322.1281	0_x000D_
-16	Polygon	44	West Hawai‘i Regional Fisheries Management Area: Kailua - Keauhou	West Hawaii Regional FMA: Kailua-Keauhou	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#west-hawaii-regional-fishery-management-area	HAR 13-60.4	The West Hawai‘i Regional Fishery Management Area (FRA) extends along the west coast of the Island of Hawaii from Ka Lae, Ka‘ū (South Point) to ‘Upolu Point, North Kohala, and from the highwater mark on shore seaward to the limit of the State’s	All types of fishing, except as indicated in prohibited activities below.	To take, kill, possess, sell, or offer for sale, any specimen of the following: Hawaiian stingray, broad stingray, pelagic stingray, spotted eagle ray, blacktip reef shark, gray reef shark, whitetip reef shark, tiger shark, whale shark, horned helmet, an	http://dlnr.hawaii.gov/dar/files/2014/05/ch60.4.pdf	N/A	FMA	Fish Replenishment Area	{a35be42b-dcf1-4769-b227-01056d230d16}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	30974930.5225	0_x000D_
-17	Polygon	19	Keauhou Bay Fisheries Management Area	Keauhou Bay FMA	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#keauhou-bay	HAR 13-57	The Keauhou Bay Fisheries Management Area is that portion of the bay bounded by a straight line drawn from Haiku‘ua Point to Kaukala‘ela‘e Point.	To take any legal size fish in season with not more than two lines at the same time. To use hand nets not exceeding three feet in any dimension to take shrimp for bait purposes only, or to land fish already hooked. To use thrownets in the zone bounded by	To snag or attempt to snag any fish. To use or possess nets, except as indicated in permitted activities above. To herd or chase any fish out of the area by swimming, diving or using a boat. To engage or attempt to engage in fish feeding.	http://dlnr.hawaii.gov/dar/files/2014/05/ch57.pdf	N/A	FMA	Fisheries Management Area	{35bd032b-2980-43b0-8f67-0ee2491fec58}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	78118.543006	0_x000D_
-18	Polygon	46	West Hawai‘i Regional Fisheries Management Area: Nāpo‘opo‘o - Hōnaunau	West Hawaii Regional FMA: Napoopoo-Hona	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#west-hawaii-regional-fishery-management-area	HAR 13-60.4	The West Hawai‘i Regional Fishery Management Area (FRA) extends along the west coast of the Island of Hawaii from Ka Lae, Ka‘ū (South Point) to ‘Upolu Point, North Kohala, and from the highwater mark on shore seaward to the limit of the State’s	All types of fishing, except as indicated in prohibited activities below.	To take, kill, possess, sell, or offer for sale, any specimen of the following: Hawaiian stingray, broad stingray, pelagic stingray, spotted eagle ray, blacktip reef shark, gray reef shark, whitetip reef shark, tiger shark, whale shark, horned helmet, an	http://dlnr.hawaii.gov/dar/files/2014/05/ch60.4.pdf	N/A	FMA	Fish Replenishment Area	{1be7f5ca-6a4a-42e2-959d-c0c73a4bc1eb}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	8197050.92045	0_x000D_
-19	Polygon	20	South Kona (Miloli‘i) ‘Opelu Management Area	South Kona Opelu Mgmt Area	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#south-kona-milolii	HAR 13-95-18, HRS 188-22.7	The waters off the coast of South Kona between the Ki‘ilae-Kēōkea boundary and the Kapua-Kaulanamauna boundary.	N/A	To fish for or take opelu with fish or animal bait, except with hook and line.	http://dlnr.hawaii.gov/dar/files/2016/03/ch95.pdf	http://www.capitol.hawaii.gov/hrscurrent/Vol03_Ch0121-0200D/HRS0188/HRS_0188-0022_0007.htm	FMA	Opelu Management Area	{add90ebb-5d87-4dad-9c54-c88ca170499c}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	24866322.1281	0_x000D_
-20	Polygon	57	West Hawai‘i Regional Fisheries Management Area: Ka‘ohe Beach	West Hawaii Regional FMA: Kaohe Beach	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#west-hawaii-regional-fishery-management-area	HAR 13-60.4	The West Hawai‘i Regional Fishery Management Area (FRA) extends along the west coast of the Island of Hawaii from Ka Lae, Ka‘ū (South Point) to ‘Upolu Point, North Kohala, and from the highwater mark on shore seaward to the limit of the State’s	All types of fishing, except as indicated in prohibited activities below.	To take, kill, possess, sell, or offer for sale, any specimen of the following: Hawaiian stingray, broad stingray, pelagic stingray, spotted eagle ray, blacktip reef shark, gray reef shark, whitetip reef shark, tiger shark, whale shark, horned helmet, an	http://dlnr.hawaii.gov/dar/files/2014/05/ch60.4.pdf	N/A	FMA	Fish Replenishment Area	{3c0cec63-1ce4-4bad-8f1a-ff6fba11494a}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	505984.894229	0_x000D_
-21	Polygon	20	South Kona (Miloli‘i) ‘Opelu Management Area	South Kona Opelu Mgmt Area	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#south-kona-milolii	HAR 13-95-18, HRS 188-22.7	The waters off the coast of South Kona between the Ki‘ilae-Kēōkea boundary and the Kapua-Kaulanamauna boundary.	N/A	To fish for or take opelu with fish or animal bait, except with hook and line.	http://dlnr.hawaii.gov/dar/files/2016/03/ch95.pdf	http://www.capitol.hawaii.gov/hrscurrent/Vol03_Ch0121-0200D/HRS0188/HRS_0188-0022_0007.htm	FMA	Opelu Management Area	{add90ebb-5d87-4dad-9c54-c88ca170499c}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	24866322.1281	0_x000D_
-22	Polygon	59	West Hawai‘i Regional Fisheries Management Area: Kaloko - Honokōhau	West Hawaii Regional FMA: Kaloko-Honokohau	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#west-hawaii-regional-fishery-management-area	HAR 13-60.4	The West Hawai‘i Regional Fishery Management Area (FRA) extends along the west coast of the Island of Hawaii from Ka Lae, Ka‘ū (South Point) to ‘Upolu Point, North Kohala, and from the highwater mark on shore seaward to the limit of the State’s	All types of fishing, except as indicated in prohibited activities below.	To take, kill, possess, sell, or offer for sale, any specimen of the following: Hawaiian stingray, broad stingray, pelagic stingray, spotted eagle ray, blacktip reef shark, gray reef shark, whitetip reef shark, tiger shark, whale shark, horned helmet, an	http://dlnr.hawaii.gov/dar/files/2014/05/ch60.4.pdf	N/A	FMA	Fish Replenishment Area / Netting Restricted Area	{78495bad-925c-4749-9296-134d25eea221}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	4117611.47484	0_x000D_
+    <t>Kona Coast” refers to the following four Fisheries Management Area Zones on the southwestern portion of Hawai‘i, each bounded by two lines extending seaward at right angles from shore and marked by signs on shore: (a) the “Wawāloli Zone”, from	To catch fish in the Zones with legal fishing gear for personal consumption.	To collect any aquarium fish within the Zones. To engage in fish feeding within the Zones, except for ‘ōpelu fishing.	http://dlnr.hawaii.gov/dar/files/2014/05/ch58.pdf	N/A	FMA	Fisheries Management Area	{89c305aa-b0ed-41f5-92b0-ab311c3d5581}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	875909.246146	0
+14	Polygon	43	West Hawai‘i Regional Fisheries Management Area: Ho‘okena	West Hawaii Regional FMA: Hookena	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#west-hawaii-regional-fishery-management-area	HAR 13-60.4	The West Hawai‘i Regional Fishery Management Area (FRA) extends along the west coast of the Island of Hawaii from Ka Lae, Ka‘ū (South Point) to ‘Upolu Point, North Kohala, and from the highwater mark on shore seaward to the limit of the State’s	All types of fishing, except as indicated in prohibited activities below.	To take, kill, possess, sell, or offer for sale, any specimen of the following: Hawaiian stingray, broad stingray, pelagic stingray, spotted eagle ray, blacktip reef shark, gray reef shark, whitetip reef shark, tiger shark, whale shark, horned helmet, an	http://dlnr.hawaii.gov/dar/files/2014/05/ch60.4.pdf	N/A	FMA	Fish Replenishment Area	{001f30aa-dd58-4b6c-b2e7-1bc7cf404eb4}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	6274248.7927	0
+15	Polygon	20	South Kona (Miloli‘i) ‘Opelu Management Area	South Kona Opelu Mgmt Area	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#south-kona-milolii	HAR 13-95-18, HRS 188-22.7	The waters off the coast of South Kona between the Ki‘ilae-Kēōkea boundary and the Kapua-Kaulanamauna boundary.	N/A	To fish for or take opelu with fish or animal bait, except with hook and line.	http://dlnr.hawaii.gov/dar/files/2016/03/ch95.pdf	http://www.capitol.hawaii.gov/hrscurrent/Vol03_Ch0121-0200D/HRS0188/HRS_0188-0022_0007.htm	FMA	Opelu Management Area	{add90ebb-5d87-4dad-9c54-c88ca170499c}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	24866322.1281	0
+16	Polygon	44	West Hawai‘i Regional Fisheries Management Area: Kailua - Keauhou	West Hawaii Regional FMA: Kailua-Keauhou	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#west-hawaii-regional-fishery-management-area	HAR 13-60.4	The West Hawai‘i Regional Fishery Management Area (FRA) extends along the west coast of the Island of Hawaii from Ka Lae, Ka‘ū (South Point) to ‘Upolu Point, North Kohala, and from the highwater mark on shore seaward to the limit of the State’s	All types of fishing, except as indicated in prohibited activities below.	To take, kill, possess, sell, or offer for sale, any specimen of the following: Hawaiian stingray, broad stingray, pelagic stingray, spotted eagle ray, blacktip reef shark, gray reef shark, whitetip reef shark, tiger shark, whale shark, horned helmet, an	http://dlnr.hawaii.gov/dar/files/2014/05/ch60.4.pdf	N/A	FMA	Fish Replenishment Area	{a35be42b-dcf1-4769-b227-01056d230d16}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	30974930.5225	0
+17	Polygon	19	Keauhou Bay Fisheries Management Area	Keauhou Bay FMA	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#keauhou-bay	HAR 13-57	The Keauhou Bay Fisheries Management Area is that portion of the bay bounded by a straight line drawn from Haiku‘ua Point to Kaukala‘ela‘e Point.	To take any legal size fish in season with not more than two lines at the same time. To use hand nets not exceeding three feet in any dimension to take shrimp for bait purposes only, or to land fish already hooked. To use thrownets in the zone bounded by	To snag or attempt to snag any fish. To use or possess nets, except as indicated in permitted activities above. To herd or chase any fish out of the area by swimming, diving or using a boat. To engage or attempt to engage in fish feeding.	http://dlnr.hawaii.gov/dar/files/2014/05/ch57.pdf	N/A	FMA	Fisheries Management Area	{35bd032b-2980-43b0-8f67-0ee2491fec58}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	78118.543006	0
+18	Polygon	46	West Hawai‘i Regional Fisheries Management Area: Nāpo‘opo‘o - Hōnaunau	West Hawaii Regional FMA: Napoopoo-Hona	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#west-hawaii-regional-fishery-management-area	HAR 13-60.4	The West Hawai‘i Regional Fishery Management Area (FRA) extends along the west coast of the Island of Hawaii from Ka Lae, Ka‘ū (South Point) to ‘Upolu Point, North Kohala, and from the highwater mark on shore seaward to the limit of the State’s	All types of fishing, except as indicated in prohibited activities below.	To take, kill, possess, sell, or offer for sale, any specimen of the following: Hawaiian stingray, broad stingray, pelagic stingray, spotted eagle ray, blacktip reef shark, gray reef shark, whitetip reef shark, tiger shark, whale shark, horned helmet, an	http://dlnr.hawaii.gov/dar/files/2014/05/ch60.4.pdf	N/A	FMA	Fish Replenishment Area	{1be7f5ca-6a4a-42e2-959d-c0c73a4bc1eb}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	8197050.92045	0
+19	Polygon	20	South Kona (Miloli‘i) ‘Opelu Management Area	South Kona Opelu Mgmt Area	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#south-kona-milolii	HAR 13-95-18, HRS 188-22.7	The waters off the coast of South Kona between the Ki‘ilae-Kēōkea boundary and the Kapua-Kaulanamauna boundary.	N/A	To fish for or take opelu with fish or animal bait, except with hook and line.	http://dlnr.hawaii.gov/dar/files/2016/03/ch95.pdf	http://www.capitol.hawaii.gov/hrscurrent/Vol03_Ch0121-0200D/HRS0188/HRS_0188-0022_0007.htm	FMA	Opelu Management Area	{add90ebb-5d87-4dad-9c54-c88ca170499c}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	24866322.1281	0
+20	Polygon	57	West Hawai‘i Regional Fisheries Management Area: Ka‘ohe Beach	West Hawaii Regional FMA: Kaohe Beach	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#west-hawaii-regional-fishery-management-area	HAR 13-60.4	The West Hawai‘i Regional Fishery Management Area (FRA) extends along the west coast of the Island of Hawaii from Ka Lae, Ka‘ū (South Point) to ‘Upolu Point, North Kohala, and from the highwater mark on shore seaward to the limit of the State’s	All types of fishing, except as indicated in prohibited activities below.	To take, kill, possess, sell, or offer for sale, any specimen of the following: Hawaiian stingray, broad stingray, pelagic stingray, spotted eagle ray, blacktip reef shark, gray reef shark, whitetip reef shark, tiger shark, whale shark, horned helmet, an	http://dlnr.hawaii.gov/dar/files/2014/05/ch60.4.pdf	N/A	FMA	Fish Replenishment Area	{3c0cec63-1ce4-4bad-8f1a-ff6fba11494a}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	505984.894229	0
+21	Polygon	20	South Kona (Miloli‘i) ‘Opelu Management Area	South Kona Opelu Mgmt Area	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#south-kona-milolii	HAR 13-95-18, HRS 188-22.7	The waters off the coast of South Kona between the Ki‘ilae-Kēōkea boundary and the Kapua-Kaulanamauna boundary.	N/A	To fish for or take opelu with fish or animal bait, except with hook and line.	http://dlnr.hawaii.gov/dar/files/2016/03/ch95.pdf	http://www.capitol.hawaii.gov/hrscurrent/Vol03_Ch0121-0200D/HRS0188/HRS_0188-0022_0007.htm	FMA	Opelu Management Area	{add90ebb-5d87-4dad-9c54-c88ca170499c}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	24866322.1281	0
+22	Polygon	59	West Hawai‘i Regional Fisheries Management Area: Kaloko - Honokōhau	West Hawaii Regional FMA: Kaloko-Honokohau	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#west-hawaii-regional-fishery-management-area	HAR 13-60.4	The West Hawai‘i Regional Fishery Management Area (FRA) extends along the west coast of the Island of Hawaii from Ka Lae, Ka‘ū (South Point) to ‘Upolu Point, North Kohala, and from the highwater mark on shore seaward to the limit of the State’s	All types of fishing, except as indicated in prohibited activities below.	To take, kill, possess, sell, or offer for sale, any specimen of the following: Hawaiian stingray, broad stingray, pelagic stingray, spotted eagle ray, blacktip reef shark, gray reef shark, whitetip reef shark, tiger shark, whale shark, horned helmet, an	http://dlnr.hawaii.gov/dar/files/2014/05/ch60.4.pdf	N/A	FMA	Fish Replenishment Area / Netting Restricted Area	{78495bad-925c-4749-9296-134d25eea221}	2016-08-05T00:00:00.000Z	dlnr_hkoike	2016-08-05T00:00:00.000Z	dlnr_hkoike	4117611.47484	0
 23	Polygon	29	Kona Coast Fisheries Management Area: Wawāloli	Kona Coast FMA: Wawaloli	http://dlnr.hawaii.gov/dar/fishing/fishing-regulations/regulated-areas/regulated-fishing-areas-on-hawaii/#kona-coast	HAR 13-58	Kona Coast” refers to the following four Fisheries Management Area Zones on the southwestern portion of Hawai‘i, each bounded by two lines extending seaward at right angles from shore and marked by signs on shore: (a) the “Wawāloli Zone”, from</t>
   </si>
   <si>
@@ -696,7 +702,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1054,16 +1060,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1128,7 +1134,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1193,7 +1199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1258,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1323,7 +1329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1388,7 +1394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1453,7 +1459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1518,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1583,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1648,7 +1654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1713,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1778,7 +1784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1843,7 +1849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1908,7 +1914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="S14" t="s">
         <v>178</v>
       </c>
@@ -1917,13 +1923,13 @@
         <v>1012069362.4742578</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="T15">
         <f>T14/T16</f>
         <v>0.37063266316908794</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="J16" t="s">
         <v>0</v>
       </c>
@@ -1949,7 +1955,7 @@
         <v>2730653455.6900001</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="J17">
         <v>0</v>
       </c>
@@ -1969,7 +1975,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="J18">
         <v>1</v>
       </c>
@@ -1993,7 +1999,7 @@
         <v>0.37063266316908794</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="S20" t="s">
         <v>207</v>
       </c>
@@ -2001,7 +2007,7 @@
         <v>457031206.809659</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>180</v>
       </c>
@@ -2039,7 +2045,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2101,9 +2107,9 @@
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2123,7 +2129,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2143,7 +2149,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2170,18 +2176,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V24"/>
+  <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
+      <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="19" max="20" width="19.42578125" customWidth="1"/>
+    <col min="19" max="20" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2246,7 +2252,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2311,7 +2317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2376,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2441,7 +2447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2506,7 +2512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2571,7 +2577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2636,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2701,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2766,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2831,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2896,7 +2902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2961,7 +2967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="409" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3026,7 +3032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="409" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3091,7 +3097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="S15" t="s">
         <v>178</v>
       </c>
@@ -3100,7 +3106,7 @@
         <v>83213132.143906012</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="S16" t="s">
         <v>179</v>
       </c>
@@ -3108,13 +3114,13 @@
         <v>2730653455.6900001</v>
       </c>
     </row>
-    <row r="17" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:23" x14ac:dyDescent="0.2">
       <c r="T17">
         <f>T15/T16</f>
         <v>3.0473706566650053E-2</v>
       </c>
     </row>
-    <row r="20" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:23" x14ac:dyDescent="0.2">
       <c r="S20" s="2" t="s">
         <v>208</v>
       </c>
@@ -3123,7 +3129,7 @@
         <v>0.12586947380412336</v>
       </c>
     </row>
-    <row r="21" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:23" x14ac:dyDescent="0.2">
       <c r="S21" s="2" t="s">
         <v>210</v>
       </c>
@@ -3131,7 +3137,7 @@
         <v>659383402.75375903</v>
       </c>
     </row>
-    <row r="23" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:23" x14ac:dyDescent="0.2">
       <c r="E23" t="s">
         <v>180</v>
       </c>
@@ -3184,7 +3190,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="24" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:23" x14ac:dyDescent="0.2">
       <c r="E24">
         <v>1</v>
       </c>
@@ -3239,6 +3245,10 @@
       <c r="V24">
         <f>SUM(G24:U24)</f>
         <v>82996241.939787999</v>
+      </c>
+      <c r="W24">
+        <f>V24/1000000</f>
+        <v>82.996241939787993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>